<commit_message>
Modified Sprint 1 Burndown Chart
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 1/Sprint 1 BurndownChart.xlsx
+++ b/Project/Phase 1/Sprint 1/Sprint 1 BurndownChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/823597be55414551/21_22/ES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Filipe\Documents\ES\jabref\Project\Phase 1\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{5687D24E-D67A-4CF1-A24E-4E16A40570FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B7F288D-439D-4C3F-9B9C-BDA3E8CE3EF7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162C9767-F88A-49A0-96C9-76556421950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,19 +427,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -516,19 +516,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1546,7 +1546,7 @@
   <dimension ref="B2:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1632,10 +1632,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -1644,10 +1644,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1657,23 +1657,23 @@
       <c r="C7" s="11"/>
       <c r="D7" s="6">
         <f>SUM(D6)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" ref="E7:I7" si="0">D7-SUM(E6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="0"/>
@@ -1687,23 +1687,23 @@
       <c r="C8" s="11"/>
       <c r="D8" s="7">
         <f>SUM(D6)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" s="7">
         <f>$D$8-($D$8/5*1)</f>
-        <v>4</v>
+        <v>5.6</v>
       </c>
       <c r="F8" s="7">
         <f>$D$8-($D$8/5*2)</f>
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="G8" s="7">
         <f>$D$8-($D$8/5*3)</f>
-        <v>2</v>
+        <v>2.8000000000000007</v>
       </c>
       <c r="H8" s="7">
         <f>$D$8-($D$8/5*4)</f>
-        <v>1</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="I8" s="7">
         <f>$D$8-($D$8/5*5)</f>

</xml_diff>